<commit_message>
Atualizacao Visual e documentacao
</commit_message>
<xml_diff>
--- a/Dados/previsao/forecast.xlsx
+++ b/Dados/previsao/forecast.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://simplenergy-my.sharepoint.com/personal/paulo_sergio_simpleenergy_com_br/Documents/Documentos/Outros/teste/Dados/previsao/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_63EB812D03A0957C123C34DA1033E7D69558990B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BA51AD1-BD76-4D1B-B39E-DE54BC45457A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="21">
   <si>
     <t>avg</t>
   </si>
@@ -81,12 +75,15 @@
   <si>
     <t>21:00:00</t>
   </si>
+  <si>
+    <t>23:00:00</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,21 +146,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -201,7 +190,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -235,7 +224,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -270,10 +258,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -446,16 +433,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -501,7 +486,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>3</v>
       </c>
@@ -524,7 +509,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2</v>
       </c>
@@ -547,7 +532,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>2</v>
       </c>
@@ -570,7 +555,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>2</v>
       </c>
@@ -593,7 +578,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>3</v>
       </c>
@@ -616,7 +601,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>3</v>
       </c>
@@ -639,7 +624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>3</v>
       </c>
@@ -662,7 +647,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>178</v>
       </c>
@@ -685,7 +670,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>146</v>
       </c>
@@ -708,7 +693,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>162</v>
       </c>
@@ -731,7 +716,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>137</v>
       </c>
@@ -754,7 +739,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>107</v>
       </c>
@@ -777,7 +762,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>106</v>
       </c>
@@ -800,7 +785,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>50</v>
       </c>
@@ -823,7 +808,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>41</v>
       </c>
@@ -846,7 +831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>103</v>
       </c>
@@ -869,7 +854,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>70</v>
       </c>
@@ -892,7 +877,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>87</v>
       </c>
@@ -915,7 +900,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>70</v>
       </c>
@@ -938,7 +923,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>58</v>
       </c>
@@ -961,7 +946,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>52</v>
       </c>
@@ -984,7 +969,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>34</v>
       </c>
@@ -1007,7 +992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>20</v>
       </c>
@@ -1030,7 +1015,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1053,7 +1038,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1076,7 +1061,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1099,7 +1084,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1122,7 +1107,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1145,7 +1130,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1168,7 +1153,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1191,7 +1176,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1214,7 +1199,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>178</v>
       </c>
@@ -1237,7 +1222,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>146</v>
       </c>
@@ -1260,7 +1245,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>162</v>
       </c>
@@ -1283,7 +1268,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>137</v>
       </c>
@@ -1306,7 +1291,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>107</v>
       </c>
@@ -1329,7 +1314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>106</v>
       </c>
@@ -1352,7 +1337,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>50</v>
       </c>
@@ -1375,7 +1360,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>41</v>
       </c>
@@ -1398,7 +1383,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>103</v>
       </c>
@@ -1421,7 +1406,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>70</v>
       </c>
@@ -1444,7 +1429,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7">
       <c r="A44">
         <v>87</v>
       </c>
@@ -1467,7 +1452,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7">
       <c r="A45">
         <v>70</v>
       </c>
@@ -1490,7 +1475,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7">
       <c r="A46">
         <v>58</v>
       </c>
@@ -1513,7 +1498,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>52</v>
       </c>
@@ -1536,7 +1521,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7">
       <c r="A48">
         <v>34</v>
       </c>
@@ -1559,7 +1544,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>20</v>
       </c>
@@ -1580,6 +1565,558 @@
       </c>
       <c r="G49" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51">
+        <v>24</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52">
+        <v>22</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53">
+        <v>24</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54">
+        <v>38</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" t="s">
+        <v>9</v>
+      </c>
+      <c r="G54" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55">
+        <v>22</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" t="s">
+        <v>9</v>
+      </c>
+      <c r="G55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56">
+        <v>3</v>
+      </c>
+      <c r="B56" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56">
+        <v>7</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57">
+        <v>8</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58">
+        <v>178</v>
+      </c>
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58">
+        <v>178</v>
+      </c>
+      <c r="D58">
+        <v>178</v>
+      </c>
+      <c r="E58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F58" t="s">
+        <v>9</v>
+      </c>
+      <c r="G58" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59">
+        <v>146</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59">
+        <v>175</v>
+      </c>
+      <c r="D59">
+        <v>68</v>
+      </c>
+      <c r="E59" t="s">
+        <v>16</v>
+      </c>
+      <c r="F59" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60">
+        <v>162</v>
+      </c>
+      <c r="B60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60">
+        <v>184</v>
+      </c>
+      <c r="D60">
+        <v>72</v>
+      </c>
+      <c r="E60" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61">
+        <v>137</v>
+      </c>
+      <c r="B61" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61">
+        <v>190</v>
+      </c>
+      <c r="D61">
+        <v>59</v>
+      </c>
+      <c r="E61" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62">
+        <v>107</v>
+      </c>
+      <c r="B62" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62">
+        <v>162</v>
+      </c>
+      <c r="D62">
+        <v>45</v>
+      </c>
+      <c r="E62" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" t="s">
+        <v>9</v>
+      </c>
+      <c r="G62" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63">
+        <v>106</v>
+      </c>
+      <c r="B63" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63">
+        <v>157</v>
+      </c>
+      <c r="D63">
+        <v>44</v>
+      </c>
+      <c r="E63" t="s">
+        <v>16</v>
+      </c>
+      <c r="F63" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64">
+        <v>50</v>
+      </c>
+      <c r="B64" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64">
+        <v>164</v>
+      </c>
+      <c r="D64">
+        <v>22</v>
+      </c>
+      <c r="E64" t="s">
+        <v>16</v>
+      </c>
+      <c r="F64" t="s">
+        <v>9</v>
+      </c>
+      <c r="G64" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65">
+        <v>41</v>
+      </c>
+      <c r="B65" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65">
+        <v>53</v>
+      </c>
+      <c r="D65">
+        <v>16</v>
+      </c>
+      <c r="E65" t="s">
+        <v>16</v>
+      </c>
+      <c r="F65" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66">
+        <v>103</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66">
+        <v>103</v>
+      </c>
+      <c r="D66">
+        <v>103</v>
+      </c>
+      <c r="E66" t="s">
+        <v>17</v>
+      </c>
+      <c r="F66" t="s">
+        <v>9</v>
+      </c>
+      <c r="G66" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67">
+        <v>70</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67">
+        <v>100</v>
+      </c>
+      <c r="D67">
+        <v>27</v>
+      </c>
+      <c r="E67" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68">
+        <v>87</v>
+      </c>
+      <c r="B68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68">
+        <v>115</v>
+      </c>
+      <c r="D68">
+        <v>30</v>
+      </c>
+      <c r="E68" t="s">
+        <v>17</v>
+      </c>
+      <c r="F68" t="s">
+        <v>9</v>
+      </c>
+      <c r="G68" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69">
+        <v>70</v>
+      </c>
+      <c r="B69" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69">
+        <v>121</v>
+      </c>
+      <c r="D69">
+        <v>25</v>
+      </c>
+      <c r="E69" t="s">
+        <v>17</v>
+      </c>
+      <c r="F69" t="s">
+        <v>9</v>
+      </c>
+      <c r="G69" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70">
+        <v>58</v>
+      </c>
+      <c r="B70" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70">
+        <v>84</v>
+      </c>
+      <c r="D70">
+        <v>30</v>
+      </c>
+      <c r="E70" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" t="s">
+        <v>9</v>
+      </c>
+      <c r="G70" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71">
+        <v>52</v>
+      </c>
+      <c r="B71" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71">
+        <v>75</v>
+      </c>
+      <c r="D71">
+        <v>15</v>
+      </c>
+      <c r="E71" t="s">
+        <v>17</v>
+      </c>
+      <c r="F71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G71" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72">
+        <v>34</v>
+      </c>
+      <c r="B72" t="s">
+        <v>13</v>
+      </c>
+      <c r="C72">
+        <v>83</v>
+      </c>
+      <c r="D72">
+        <v>14</v>
+      </c>
+      <c r="E72" t="s">
+        <v>17</v>
+      </c>
+      <c r="F72" t="s">
+        <v>9</v>
+      </c>
+      <c r="G72" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73">
+        <v>20</v>
+      </c>
+      <c r="B73" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73">
+        <v>25</v>
+      </c>
+      <c r="D73">
+        <v>10</v>
+      </c>
+      <c r="E73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F73" t="s">
+        <v>9</v>
+      </c>
+      <c r="G73" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>